<commit_message>
Fix Exam 1 scoring
</commit_message>
<xml_diff>
--- a/scicomp301-cpp-linux-syllabus.xlsx
+++ b/scicomp301-cpp-linux-syllabus.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DaveB\SciComp\Courses\scicomp301-cpp-linux\scicomp301-cpp-linux\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DaveB\SciComp\Courses\scicomp301-cpp-linux\scicomp301-cpp-linux-instructor\Supporting Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C238BD81-8C41-4756-8A1F-66032C5C3B21}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF5A8863-13E3-4832-AF96-B2AC7A9818F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22215" yWindow="1245" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Current" sheetId="3" r:id="rId1"/>
@@ -25,7 +25,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="622">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="633">
   <si>
     <t>Topics</t>
   </si>
@@ -98,12 +100,6 @@
     <t>Cryptanalysis</t>
   </si>
   <si>
-    <t>Full Adder</t>
-  </si>
-  <si>
-    <t>2-of-3 Majority Vote</t>
-  </si>
-  <si>
     <t>Moment of Distribution</t>
   </si>
   <si>
@@ -125,9 +121,6 @@
     <t>Taylor Series</t>
   </si>
   <si>
-    <t>Euler's Equation</t>
-  </si>
-  <si>
     <t>Pachinko Distribution</t>
   </si>
   <si>
@@ -185,18 +178,12 @@
     <t>Temperature Conversion</t>
   </si>
   <si>
-    <t>Trace the Circuit</t>
-  </si>
-  <si>
     <t>Sequential Circuits</t>
   </si>
   <si>
     <t>Boolean Algebra, Digital Logic Gates</t>
   </si>
   <si>
-    <t>Truth Tables</t>
-  </si>
-  <si>
     <t>Continued Fractions Taxonomy</t>
   </si>
   <si>
@@ -431,9 +418,6 @@
     <t>euler-identity</t>
   </si>
   <si>
-    <t>euler-equation</t>
-  </si>
-  <si>
     <t>scramble-squares</t>
   </si>
   <si>
@@ -1376,9 +1360,6 @@
     <t>kMeans using Manhattan Distance</t>
   </si>
   <si>
-    <t>circuits-logisim</t>
-  </si>
-  <si>
     <t>Multithreading</t>
   </si>
   <si>
@@ -1899,6 +1880,60 @@
   </si>
   <si>
     <t>collatz_conjecture</t>
+  </si>
+  <si>
+    <t>euler-formula</t>
+  </si>
+  <si>
+    <t>Euler's Formula</t>
+  </si>
+  <si>
+    <t>Combinatorial Circuit</t>
+  </si>
+  <si>
+    <t>Logisim, Truth Tables</t>
+  </si>
+  <si>
+    <t>2-of-3 Majority Vote (Logisim)</t>
+  </si>
+  <si>
+    <t>Full Adder (Logisim)</t>
+  </si>
+  <si>
+    <t>Trace the Circuit (Paper)</t>
+  </si>
+  <si>
+    <t>Circuit Simulation (Logisim)</t>
+  </si>
+  <si>
+    <t>simple-circuit-logisim</t>
+  </si>
+  <si>
+    <t>majority-vote-logisim</t>
+  </si>
+  <si>
+    <t>full-adder-logisim</t>
+  </si>
+  <si>
+    <t>simple-circuit-trace</t>
+  </si>
+  <si>
+    <t>Population vs. Sample Variance</t>
+  </si>
+  <si>
+    <t>Random Sampling, Bessel's Correction</t>
+  </si>
+  <si>
+    <t>sample-variance</t>
+  </si>
+  <si>
+    <t>Geometry of Random Sampling</t>
+  </si>
+  <si>
+    <t>surface-distribution</t>
+  </si>
+  <si>
+    <t>Radial Density in Circles and Spheres</t>
   </si>
 </sst>
 </file>
@@ -1986,7 +2021,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2078,6 +2113,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2396,11 +2437,9 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F208"/>
+  <dimension ref="A1:F209"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2415,7 +2454,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2424,16 +2463,16 @@
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="12" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -2446,7 +2485,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="E4" s="10"/>
       <c r="F4" s="29"/>
@@ -2454,25 +2493,25 @@
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
       <c r="B5" s="6" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="10"/>
       <c r="B6" s="6" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="10"/>
       <c r="B7" s="6" t="s">
-        <v>441</v>
+        <v>435</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -2480,23 +2519,23 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="E9" s="10"/>
       <c r="F9" s="29"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -2508,25 +2547,25 @@
         <v>7</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="14"/>
       <c r="B12" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -2535,7 +2574,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="E14" s="10"/>
       <c r="F14" s="29"/>
@@ -2543,91 +2582,91 @@
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="14"/>
       <c r="B15" s="6" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="14"/>
       <c r="B16" s="6" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="14"/>
       <c r="B17" s="6" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>511</v>
+        <v>504</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="14"/>
       <c r="B18" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
       <c r="B19" s="6" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="14"/>
       <c r="B20" s="6" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -2635,7 +2674,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="E22" s="10"/>
       <c r="F22" s="29"/>
@@ -2643,76 +2682,76 @@
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="14"/>
       <c r="B23" s="6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="14"/>
       <c r="B24" s="17" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="D24" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E24" s="6" t="s">
         <v>108</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="14"/>
       <c r="B25" s="6" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D25" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="E25" s="6" t="s">
         <v>109</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="14"/>
       <c r="B26" s="18" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="14"/>
       <c r="B27" s="3" t="s">
-        <v>454</v>
+        <v>447</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -2720,7 +2759,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="E29" s="19"/>
       <c r="F29" s="30"/>
@@ -2731,56 +2770,56 @@
         <v>16</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="14"/>
       <c r="B31" s="6" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B32" s="6" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B33" s="6" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -2789,13 +2828,13 @@
         <v>18</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -2803,7 +2842,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="E36" s="19"/>
       <c r="F36" s="30"/>
@@ -2811,61 +2850,61 @@
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="14"/>
       <c r="B37" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="14"/>
       <c r="B38" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C38" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C38" s="6" t="s">
-        <v>25</v>
-      </c>
       <c r="D38" s="5" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="14"/>
       <c r="B39" s="6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="14"/>
       <c r="B40" s="6" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -2873,84 +2912,84 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="E42" s="10"/>
       <c r="F42" s="29"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B43" s="6" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B44" s="6" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B45" s="6" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B46" s="6" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B47" s="6" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="10" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="B49" s="17"/>
       <c r="C49" s="17"/>
@@ -2961,16 +3000,16 @@
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="14"/>
       <c r="B50" s="6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C50" s="6" t="s">
         <v>13</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E50" s="8" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="F50" s="32"/>
     </row>
@@ -2982,10 +3021,10 @@
         <v>11</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E51" s="8" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="F51" s="32"/>
     </row>
@@ -2998,210 +3037,210 @@
         <v>12</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E52" s="8" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="F52" s="32"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="14"/>
       <c r="B53" s="6" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C53" s="18" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="11" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
       <c r="B56" s="6" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>412</v>
-      </c>
-      <c r="F56" s="5">
+        <v>406</v>
+      </c>
+      <c r="F56" s="42">
         <v>15</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
       <c r="B57" s="1" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="C57" s="18" t="s">
-        <v>420</v>
+        <v>414</v>
       </c>
       <c r="D57" s="33" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="E57" s="18" t="s">
-        <v>421</v>
-      </c>
-      <c r="F57" s="33">
-        <v>10</v>
+        <v>415</v>
+      </c>
+      <c r="F57" s="42">
+        <v>15</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
       <c r="B58" s="1" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>413</v>
-      </c>
-      <c r="F58" s="5">
+        <v>407</v>
+      </c>
+      <c r="F58" s="42">
         <v>10</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
       <c r="B59" s="1" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>424</v>
-      </c>
-      <c r="F59" s="5">
+        <v>418</v>
+      </c>
+      <c r="F59" s="42">
         <v>5</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
       <c r="B60" s="1" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="E60" s="37" t="s">
-        <v>425</v>
-      </c>
-      <c r="F60" s="5">
+        <v>419</v>
+      </c>
+      <c r="F60" s="42">
         <v>10</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
       <c r="B61" s="1" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>426</v>
-      </c>
-      <c r="F61" s="5">
+        <v>420</v>
+      </c>
+      <c r="F61" s="42">
         <v>5</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
       <c r="B62" s="1" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="E62" s="6" t="s">
-        <v>414</v>
-      </c>
-      <c r="F62" s="5">
+        <v>408</v>
+      </c>
+      <c r="F62" s="42">
         <v>5</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
       <c r="B63" s="1" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="E63" s="6" t="s">
-        <v>422</v>
-      </c>
-      <c r="F63" s="5">
-        <v>20</v>
+        <v>416</v>
+      </c>
+      <c r="F63" s="42">
+        <v>15</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
       <c r="B64" s="1" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="E64" s="6" t="s">
-        <v>423</v>
-      </c>
-      <c r="F64" s="5">
+        <v>417</v>
+      </c>
+      <c r="F64" s="42">
         <v>10</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="2"/>
       <c r="B65" s="1" t="s">
-        <v>415</v>
+        <v>409</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>416</v>
+        <v>410</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="E65" s="6" t="s">
-        <v>417</v>
-      </c>
-      <c r="F65" s="34">
+        <v>411</v>
+      </c>
+      <c r="F65" s="43">
         <v>10</v>
       </c>
     </row>
@@ -3216,7 +3255,7 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="10" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="E67" s="19"/>
       <c r="F67" s="30"/>
@@ -3224,31 +3263,31 @@
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="19"/>
       <c r="B68" s="6" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E68" s="6" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="21"/>
       <c r="B69" s="6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E69" s="6" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -3256,30 +3295,30 @@
         <v>4</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E70" s="9" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="14"/>
       <c r="B71" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E71" s="6" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="10" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="E73" s="19"/>
       <c r="F73" s="30"/>
@@ -3287,66 +3326,66 @@
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="14"/>
       <c r="B74" s="6" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E74" s="6" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="14"/>
       <c r="B75" s="6" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E75" s="6" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="14"/>
       <c r="B76" s="6" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="D76" s="5" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E76" s="6" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="14"/>
       <c r="B77" s="6" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="D77" s="5" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E77" s="6" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="10" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="E79" s="4"/>
       <c r="F79" s="29"/>
@@ -3356,85 +3395,85 @@
         <v>2</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="D80" s="5" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E80" s="6" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B81" s="22" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="C81" s="22" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="D81" s="7" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E81" s="8" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="F81" s="32"/>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B82" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C82" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D82" s="5" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E82" s="6" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B83" s="6" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>30</v>
+        <v>616</v>
       </c>
       <c r="D83" s="5" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E83" s="6" t="s">
-        <v>132</v>
+        <v>615</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B84" s="6" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="E84" s="6" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="6"/>
       <c r="B85" s="6" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="C85" s="6" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="D85" s="5" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="E85" s="6" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -3443,7 +3482,7 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="10" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="B87" s="17"/>
       <c r="C87" s="17"/>
@@ -3454,58 +3493,58 @@
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="14"/>
       <c r="B88" s="6" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C88" s="6" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D88" s="5" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E88" s="6" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B89" s="6" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C89" s="6" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D89" s="5" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E89" s="6" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B90" s="6" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="C90" s="6" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="D90" s="5" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E90" s="6" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B91" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C91" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C91" s="6" t="s">
-        <v>31</v>
-      </c>
       <c r="D91" s="5" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E91" s="6" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
@@ -3513,7 +3552,7 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="10" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="E93" s="19"/>
       <c r="F93" s="30"/>
@@ -3521,46 +3560,46 @@
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="19"/>
       <c r="B94" s="6" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C94" s="6" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D94" s="5" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E94" s="6" t="s">
-        <v>619</v>
+        <v>612</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="19"/>
       <c r="B95" s="6" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C95" s="6" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D95" s="5" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E95" s="6" t="s">
-        <v>620</v>
+        <v>613</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="19"/>
       <c r="B96" s="6" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C96" s="6" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D96" s="5" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E96" s="6" t="s">
-        <v>621</v>
+        <v>614</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
@@ -3568,7 +3607,7 @@
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="10" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="E98" s="19"/>
       <c r="F98" s="30"/>
@@ -3576,46 +3615,46 @@
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="19"/>
       <c r="B99" s="6" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="C99" s="6" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="D99" s="5" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E99" s="8" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="F99" s="32"/>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B100" s="6" t="s">
-        <v>432</v>
+        <v>426</v>
       </c>
       <c r="C100" s="9" t="s">
-        <v>431</v>
+        <v>425</v>
       </c>
       <c r="D100" s="5" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E100" s="6" t="s">
-        <v>429</v>
+        <v>423</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="14"/>
       <c r="B101" s="6" t="s">
-        <v>433</v>
+        <v>427</v>
       </c>
       <c r="C101" s="9" t="s">
-        <v>434</v>
+        <v>428</v>
       </c>
       <c r="D101" s="5" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E101" s="6" t="s">
-        <v>429</v>
+        <v>423</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
@@ -3624,73 +3663,73 @@
         <v>20</v>
       </c>
       <c r="C102" s="6" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D102" s="5" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E102" s="6" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="14"/>
       <c r="B103" s="6" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C103" s="6" t="s">
         <v>19</v>
       </c>
       <c r="D103" s="5" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E103" s="6" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="14"/>
       <c r="B104" s="6" t="s">
-        <v>612</v>
+        <v>605</v>
       </c>
       <c r="C104" s="6" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="D104" s="5" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="E104" s="6" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="14"/>
       <c r="B105" s="6" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="C105" s="6" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="D105" s="5" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="E105" s="6" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="14"/>
       <c r="B106" s="6" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="C106" s="6" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="D106" s="5" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="E106" s="6" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
@@ -3698,7 +3737,7 @@
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="10" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="E108" s="19"/>
       <c r="F108" s="30"/>
@@ -3709,28 +3748,28 @@
         <v>5</v>
       </c>
       <c r="C109" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D109" s="5" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E109" s="6" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="14"/>
       <c r="B110" s="6" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C110" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D110" s="5" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E110" s="6" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
@@ -3738,7 +3777,7 @@
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="10" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="E112" s="19"/>
       <c r="F112" s="30"/>
@@ -3746,91 +3785,91 @@
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="14"/>
       <c r="B113" s="6" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="C113" s="6" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="D113" s="5" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E113" s="6" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="14"/>
       <c r="B114" s="6" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="C114" s="6" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D114" s="5" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E114" s="6" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="14"/>
       <c r="B115" s="6" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="C115" s="6" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D115" s="5" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E115" s="6" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="14"/>
       <c r="B116" s="6" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="C116" s="6" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D116" s="5" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E116" s="6" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="14"/>
       <c r="B117" s="6" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="C117" s="6" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D117" s="5" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E117" s="6" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="14"/>
       <c r="B118" s="6" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="C118" s="6" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D118" s="5" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="E118" s="6" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
@@ -3838,7 +3877,7 @@
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" s="10" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="E120" s="19"/>
       <c r="F120" s="30"/>
@@ -3846,31 +3885,31 @@
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="14"/>
       <c r="B121" s="6" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C121" s="6" t="s">
         <v>1</v>
       </c>
       <c r="D121" s="5" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E121" s="6" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="14"/>
       <c r="B122" s="6" t="s">
-        <v>443</v>
+        <v>437</v>
       </c>
       <c r="C122" s="28" t="s">
-        <v>444</v>
+        <v>438</v>
       </c>
       <c r="D122" s="5" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E122" s="6" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
@@ -3878,7 +3917,7 @@
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="10" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="E124" s="19"/>
       <c r="F124" s="30"/>
@@ -3886,62 +3925,62 @@
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="14"/>
       <c r="B125" s="6" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="C125" s="18" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D125" s="5" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E125" s="18" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="F125" s="33"/>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" s="14"/>
       <c r="B126" s="6" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C126" s="18" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D126" s="5" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E126" s="6" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" s="14"/>
       <c r="B127" s="6" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C127" s="18" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D127" s="5" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E127" s="6" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" s="14"/>
       <c r="B128" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C128" s="6" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D128" s="5" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E128" s="6" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
@@ -3949,22 +3988,22 @@
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" s="11" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" s="11"/>
       <c r="B131" s="6" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="C131" s="6" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="D131" s="5" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="E131" s="6" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="F131" s="5">
         <v>5</v>
@@ -3973,52 +4012,52 @@
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" s="11"/>
       <c r="B132" s="6" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="C132" s="6" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="D132" s="5" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="E132" s="6" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="F132" s="5">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" s="11"/>
       <c r="B133" s="6" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="C133" s="6" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="D133" s="5" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="E133" s="6" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="F133" s="5">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" s="11"/>
       <c r="B134" s="6" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="C134" s="6" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="D134" s="5" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="E134" s="6" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="F134" s="5">
         <v>10</v>
@@ -4027,16 +4066,16 @@
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" s="11"/>
       <c r="B135" s="6" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="C135" s="6" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D135" s="5" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="E135" s="6" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="F135" s="5">
         <v>15</v>
@@ -4045,16 +4084,16 @@
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" s="11"/>
       <c r="B136" s="6" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="C136" s="6" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="D136" s="5" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="E136" s="6" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="F136" s="5">
         <v>10</v>
@@ -4063,16 +4102,16 @@
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" s="11"/>
       <c r="B137" s="6" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
       <c r="C137" s="6" t="s">
-        <v>430</v>
+        <v>424</v>
       </c>
       <c r="D137" s="5" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="E137" s="6" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="F137" s="5">
         <v>5</v>
@@ -4081,16 +4120,16 @@
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" s="11"/>
       <c r="B138" s="6" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="C138" s="6" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="D138" s="5" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="E138" s="6" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="F138" s="5">
         <v>10</v>
@@ -4099,16 +4138,16 @@
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" s="11"/>
       <c r="B139" s="6" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="C139" s="6" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="D139" s="5" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="E139" s="6" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="F139" s="5">
         <v>5</v>
@@ -4117,16 +4156,16 @@
     <row r="140" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A140" s="11"/>
       <c r="B140" s="6" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C140" s="6" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D140" s="5" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="E140" s="6" t="s">
-        <v>436</v>
+        <v>430</v>
       </c>
       <c r="F140" s="34">
         <v>5</v>
@@ -4141,7 +4180,7 @@
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" s="10" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="B142" s="17"/>
       <c r="C142" s="17"/>
@@ -4151,76 +4190,76 @@
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B143" s="6" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C143" s="6" t="s">
         <v>3</v>
       </c>
       <c r="D143" s="5" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E143" s="6" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" s="14"/>
       <c r="B144" s="6" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C144" s="6" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D144" s="5" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E144" s="6" t="s">
-        <v>437</v>
+        <v>431</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" s="14"/>
       <c r="B145" s="6" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C145" s="6" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D145" s="5" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E145" s="6" t="s">
-        <v>438</v>
+        <v>432</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" s="14"/>
       <c r="B146" s="6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C146" s="6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D146" s="5" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E146" s="6" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" s="14"/>
       <c r="B147" s="6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C147" s="6" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D147" s="5" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="E147" s="6" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.25">
@@ -4229,7 +4268,7 @@
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" s="10" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="E149" s="19"/>
       <c r="F149" s="30"/>
@@ -4237,91 +4276,91 @@
     <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" s="23"/>
       <c r="B150" s="6" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C150" s="6" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D150" s="5" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E150" s="6" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" s="23"/>
       <c r="B151" s="6" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C151" s="6" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D151" s="5" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E151" s="6" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" s="23"/>
       <c r="B152" s="6" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C152" s="6" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D152" s="5" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E152" s="6" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" s="23"/>
       <c r="B153" s="6" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C153" s="6" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D153" s="5" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E153" s="6" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" s="23"/>
       <c r="B154" s="17" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="C154" s="17" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="D154" s="5" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="E154" s="6" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" s="23"/>
       <c r="B155" s="8" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="C155" s="8" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="D155" s="5" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="E155" s="6" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
@@ -4330,7 +4369,7 @@
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" s="10" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="E157" s="19"/>
       <c r="F157" s="30"/>
@@ -4338,62 +4377,62 @@
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" s="14"/>
       <c r="B158" s="6" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="C158" s="6" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="D158" s="5" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E158" s="6" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159" s="14"/>
       <c r="B159" s="25" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="C159" s="25" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="D159" s="5" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E159" s="6" t="s">
-        <v>439</v>
+        <v>433</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160" s="14"/>
       <c r="B160" s="25" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="C160" s="25" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="D160" s="5" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E160" s="8" t="s">
-        <v>615</v>
+        <v>608</v>
       </c>
       <c r="F160" s="32"/>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161" s="14"/>
       <c r="B161" s="25" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="C161" s="25" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="D161" s="5" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E161" s="6" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.25">
@@ -4402,51 +4441,51 @@
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163" s="10" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="E163" s="10"/>
       <c r="F163" s="29"/>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B164" s="6" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="C164" s="6" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="D164" s="5" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E164" s="6" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B165" s="6" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="C165" s="6" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="D165" s="5" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E165" s="6" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B166" s="6" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="C166" s="6" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="D166" s="5" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E166" s="6" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
@@ -4459,83 +4498,83 @@
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168" s="10" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="E168" s="10"/>
       <c r="F168" s="29"/>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B169" s="6" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="C169" s="6" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="D169" s="5" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E169" s="8" t="s">
-        <v>440</v>
+        <v>434</v>
       </c>
       <c r="F169" s="32"/>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B170" s="6" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="C170" s="6" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="D170" s="5" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E170" s="8" t="s">
-        <v>440</v>
+        <v>434</v>
       </c>
       <c r="F170" s="32"/>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B171" s="6" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="C171" s="6" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="D171" s="5" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E171" s="8" t="s">
-        <v>440</v>
+        <v>434</v>
       </c>
       <c r="F171" s="32"/>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B172" s="6" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="C172" s="6" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="D172" s="5" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E172" s="8" t="s">
-        <v>440</v>
+        <v>434</v>
       </c>
       <c r="F172" s="32"/>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B173" s="6" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="C173" s="6" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="D173" s="5" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="E173" s="6" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.25">
@@ -4548,114 +4587,114 @@
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A175" s="10" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="E175" s="10"/>
       <c r="F175" s="29"/>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B176" s="6" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="C176" s="6" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="D176" s="5" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E176" s="6" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B177" s="6" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="C177" s="6" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="D177" s="5" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E177" s="6" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A178" s="14"/>
       <c r="B178" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C178" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C178" s="6" t="s">
-        <v>43</v>
-      </c>
       <c r="D178" s="5" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E178" s="6" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B179" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C179" s="6" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="D179" s="5" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E179" s="6" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B180" s="6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C180" s="6" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="D180" s="5" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="E180" s="6" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B181" s="6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C181" s="6" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D181" s="5" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="E181" s="6" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A183" s="11" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A184" s="11"/>
       <c r="B184" s="6" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="C184" s="6" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
       <c r="D184" s="5" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="E184" s="6" t="s">
-        <v>616</v>
+        <v>609</v>
       </c>
       <c r="F184" s="5">
         <v>10</v>
@@ -4664,16 +4703,16 @@
     <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A185" s="11"/>
       <c r="B185" s="6" t="s">
-        <v>406</v>
+        <v>400</v>
       </c>
       <c r="C185" s="6" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
       <c r="D185" s="5" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="E185" s="6" t="s">
-        <v>617</v>
+        <v>610</v>
       </c>
       <c r="F185" s="5">
         <v>15</v>
@@ -4682,16 +4721,16 @@
     <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A186" s="11"/>
       <c r="B186" s="6" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="C186" s="6" t="s">
-        <v>398</v>
+        <v>392</v>
       </c>
       <c r="D186" s="5" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="E186" s="6" t="s">
-        <v>618</v>
+        <v>611</v>
       </c>
       <c r="F186" s="5">
         <v>15</v>
@@ -4700,16 +4739,16 @@
     <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A187" s="11"/>
       <c r="B187" s="6" t="s">
-        <v>407</v>
+        <v>401</v>
       </c>
       <c r="C187" s="6" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="D187" s="5" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="E187" s="6" t="s">
-        <v>399</v>
+        <v>393</v>
       </c>
       <c r="F187" s="5">
         <v>10</v>
@@ -4718,16 +4757,16 @@
     <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A188" s="11"/>
       <c r="B188" s="6" t="s">
-        <v>410</v>
+        <v>404</v>
       </c>
       <c r="C188" s="6" t="s">
-        <v>395</v>
+        <v>389</v>
       </c>
       <c r="D188" s="5" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="E188" s="6" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
       <c r="F188" s="5">
         <v>10</v>
@@ -4736,16 +4775,16 @@
     <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A189" s="11"/>
       <c r="B189" s="6" t="s">
-        <v>409</v>
+        <v>403</v>
       </c>
       <c r="C189" s="6" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="D189" s="5" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="E189" s="6" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="F189" s="5">
         <v>15</v>
@@ -4754,16 +4793,16 @@
     <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A190" s="11"/>
       <c r="B190" s="6" t="s">
-        <v>408</v>
+        <v>402</v>
       </c>
       <c r="C190" s="6" t="s">
-        <v>411</v>
+        <v>405</v>
       </c>
       <c r="D190" s="5" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="E190" s="6" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="F190" s="5">
         <v>5</v>
@@ -4772,16 +4811,16 @@
     <row r="191" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A191" s="11"/>
       <c r="B191" s="6" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="C191" s="6" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="D191" s="5" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="E191" s="6" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="F191" s="5">
         <v>15</v>
@@ -4790,16 +4829,16 @@
     <row r="192" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A192" s="11"/>
       <c r="B192" s="6" t="s">
-        <v>443</v>
+        <v>437</v>
       </c>
       <c r="C192" s="6" t="s">
-        <v>446</v>
+        <v>440</v>
       </c>
       <c r="D192" s="5" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="E192" s="6" t="s">
-        <v>445</v>
+        <v>439</v>
       </c>
       <c r="F192" s="34">
         <v>5</v>
@@ -4814,38 +4853,38 @@
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194" s="10" t="s">
-        <v>427</v>
+        <v>421</v>
       </c>
       <c r="E194" s="10"/>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A195" s="23"/>
       <c r="B195" s="26" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="C195" s="26" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="D195" s="27" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E195" s="28" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A196" s="14"/>
       <c r="B196" s="26" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="C196" s="26" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="D196" s="27" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E196" s="28" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.25">
@@ -4853,133 +4892,147 @@
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198" s="10" t="s">
-        <v>428</v>
+        <v>422</v>
       </c>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B199" s="6" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C199" s="6" t="s">
-        <v>50</v>
+        <v>621</v>
       </c>
       <c r="D199" s="5" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E199" s="6" t="s">
-        <v>79</v>
+        <v>626</v>
       </c>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B200" s="6" t="s">
-        <v>53</v>
+        <v>617</v>
       </c>
       <c r="C200" s="6" t="s">
-        <v>22</v>
+        <v>622</v>
       </c>
       <c r="D200" s="5" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E200" s="6" t="s">
-        <v>447</v>
+        <v>623</v>
       </c>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B201" s="6" t="s">
-        <v>51</v>
+        <v>618</v>
       </c>
       <c r="C201" s="6" t="s">
-        <v>21</v>
+        <v>619</v>
       </c>
       <c r="D201" s="5" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E201" s="6" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A203" s="40" t="s">
-        <v>442</v>
-      </c>
-      <c r="B203" s="18"/>
-      <c r="C203" s="18"/>
-      <c r="D203" s="33"/>
-      <c r="E203" s="40"/>
+        <v>624</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B202" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C202" s="6" t="s">
+        <v>620</v>
+      </c>
+      <c r="D202" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="E202" s="6" t="s">
+        <v>625</v>
+      </c>
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A204" s="41"/>
-      <c r="B204" s="18" t="s">
-        <v>448</v>
-      </c>
-      <c r="C204" s="18" t="s">
-        <v>264</v>
-      </c>
-      <c r="D204" s="33" t="s">
-        <v>107</v>
-      </c>
-      <c r="E204" s="18" t="s">
-        <v>259</v>
-      </c>
+      <c r="A204" s="40" t="s">
+        <v>436</v>
+      </c>
+      <c r="B204" s="18"/>
+      <c r="C204" s="18"/>
+      <c r="D204" s="33"/>
+      <c r="E204" s="40"/>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A205" s="41"/>
       <c r="B205" s="18" t="s">
-        <v>314</v>
+        <v>441</v>
       </c>
       <c r="C205" s="18" t="s">
-        <v>450</v>
+        <v>258</v>
       </c>
       <c r="D205" s="33" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="E205" s="18" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A206" s="41"/>
       <c r="B206" s="18" t="s">
-        <v>449</v>
+        <v>308</v>
       </c>
       <c r="C206" s="18" t="s">
-        <v>265</v>
+        <v>443</v>
       </c>
       <c r="D206" s="33" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="E206" s="18" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A207" s="41"/>
       <c r="B207" s="18" t="s">
-        <v>266</v>
-      </c>
-      <c r="C207" s="6" t="s">
-        <v>451</v>
+        <v>442</v>
+      </c>
+      <c r="C207" s="18" t="s">
+        <v>259</v>
       </c>
       <c r="D207" s="33" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="E207" s="18" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A208" s="41"/>
       <c r="B208" s="18" t="s">
-        <v>456</v>
-      </c>
-      <c r="C208" s="18" t="s">
-        <v>267</v>
+        <v>260</v>
+      </c>
+      <c r="C208" s="6" t="s">
+        <v>444</v>
       </c>
       <c r="D208" s="33" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="E208" s="18" t="s">
-        <v>263</v>
+        <v>255</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A209" s="41"/>
+      <c r="B209" s="18" t="s">
+        <v>449</v>
+      </c>
+      <c r="C209" s="18" t="s">
+        <v>261</v>
+      </c>
+      <c r="D209" s="33" t="s">
+        <v>114</v>
+      </c>
+      <c r="E209" s="18" t="s">
+        <v>257</v>
       </c>
     </row>
   </sheetData>
@@ -4996,9 +5049,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F96"/>
+  <dimension ref="A1:F98"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="G52" sqref="G52"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5013,7 +5068,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="B1" s="18"/>
       <c r="C1" s="18"/>
@@ -5023,137 +5078,137 @@
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
       <c r="B2" s="18" t="s">
-        <v>457</v>
+        <v>450</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>459</v>
+        <v>452</v>
       </c>
       <c r="D2" s="33" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>458</v>
+        <v>451</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="10"/>
       <c r="B3" s="18" t="s">
-        <v>467</v>
+        <v>460</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="D3" s="33" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>469</v>
+        <v>462</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="10"/>
       <c r="B4" s="18" t="s">
-        <v>477</v>
+        <v>470</v>
       </c>
       <c r="C4" s="18"/>
       <c r="D4" s="33" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>478</v>
+        <v>471</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="41"/>
       <c r="B5" s="18" t="s">
-        <v>463</v>
+        <v>456</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>464</v>
+        <v>457</v>
       </c>
       <c r="D5" s="33" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>512</v>
+        <v>505</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>492</v>
+        <v>485</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="10"/>
       <c r="B8" s="6" t="s">
-        <v>513</v>
+        <v>506</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>514</v>
+        <v>507</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>604</v>
+        <v>597</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="10"/>
       <c r="B9" s="6" t="s">
-        <v>515</v>
+        <v>508</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>516</v>
+        <v>509</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>605</v>
+        <v>598</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
       <c r="B10" s="6" t="s">
-        <v>452</v>
+        <v>445</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>453</v>
+        <v>446</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>455</v>
+        <v>448</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" s="35" t="s">
-        <v>519</v>
+        <v>512</v>
       </c>
       <c r="C11" s="35" t="s">
-        <v>520</v>
+        <v>513</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E11" s="36" t="s">
-        <v>418</v>
+        <v>412</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" s="35" t="s">
-        <v>419</v>
+        <v>413</v>
       </c>
       <c r="C12" s="35" t="s">
-        <v>518</v>
+        <v>511</v>
       </c>
       <c r="D12" s="27" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="E12" s="36" t="s">
-        <v>517</v>
+        <v>510</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -5165,7 +5220,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
-        <v>505</v>
+        <v>498</v>
       </c>
       <c r="C14" s="18"/>
       <c r="D14" s="33"/>
@@ -5174,73 +5229,73 @@
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
       <c r="B15" s="6" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="D15" s="33" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>498</v>
+        <v>491</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" s="28" t="s">
-        <v>521</v>
+        <v>514</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>522</v>
+        <v>515</v>
       </c>
       <c r="D16" s="33" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>497</v>
+        <v>490</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B17" s="28" t="s">
-        <v>523</v>
+        <v>516</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>524</v>
+        <v>517</v>
       </c>
       <c r="D17" s="33" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>500</v>
+        <v>493</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B18" s="6" t="s">
-        <v>525</v>
+        <v>518</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>526</v>
+        <v>519</v>
       </c>
       <c r="D18" s="33" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>483</v>
+        <v>476</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="41"/>
       <c r="B19" s="18" t="s">
-        <v>614</v>
+        <v>607</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>527</v>
+        <v>520</v>
       </c>
       <c r="D19" s="33" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>488</v>
+        <v>481</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -5251,7 +5306,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
-        <v>501</v>
+        <v>494</v>
       </c>
       <c r="B21" s="18"/>
       <c r="C21" s="18"/>
@@ -5265,97 +5320,97 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
-        <v>506</v>
+        <v>499</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="10"/>
       <c r="B24" s="6" t="s">
-        <v>529</v>
+        <v>522</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>528</v>
+        <v>521</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>491</v>
+        <v>484</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="10"/>
       <c r="B25" s="6" t="s">
-        <v>530</v>
+        <v>523</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>531</v>
+        <v>524</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>490</v>
+        <v>483</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="10"/>
       <c r="B26" s="6" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>532</v>
+        <v>525</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>606</v>
+        <v>599</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="10"/>
       <c r="B27" s="6" t="s">
-        <v>534</v>
+        <v>527</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>535</v>
+        <v>528</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>607</v>
+        <v>600</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="10"/>
       <c r="B28" s="6" t="s">
-        <v>536</v>
+        <v>529</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>537</v>
+        <v>530</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>476</v>
+        <v>469</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="10"/>
       <c r="B29" s="6" t="s">
-        <v>538</v>
+        <v>531</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>539</v>
+        <v>532</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>608</v>
+        <v>601</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -5363,82 +5418,82 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
-        <v>543</v>
+        <v>536</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="10"/>
       <c r="B32" s="6" t="s">
-        <v>496</v>
+        <v>489</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>540</v>
+        <v>533</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>481</v>
+        <v>474</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="10"/>
       <c r="B33" s="6" t="s">
-        <v>541</v>
+        <v>534</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>542</v>
+        <v>535</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>482</v>
+        <v>475</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="10"/>
       <c r="B34" s="6" t="s">
-        <v>545</v>
+        <v>538</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>546</v>
+        <v>539</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E34" s="18" t="s">
-        <v>544</v>
+        <v>537</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="41"/>
       <c r="B35" s="18" t="s">
-        <v>485</v>
+        <v>478</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>549</v>
+        <v>542</v>
       </c>
       <c r="D35" s="33" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>486</v>
+        <v>479</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="41"/>
       <c r="B36" s="18" t="s">
-        <v>547</v>
+        <v>540</v>
       </c>
       <c r="C36" s="18" t="s">
-        <v>548</v>
+        <v>541</v>
       </c>
       <c r="D36" s="33" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>487</v>
+        <v>480</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -5449,444 +5504,466 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
-        <v>507</v>
+        <v>500</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="10"/>
       <c r="B39" s="6" t="s">
-        <v>551</v>
+        <v>544</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>550</v>
+        <v>543</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>461</v>
+        <v>454</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="10"/>
       <c r="B40" s="6" t="s">
-        <v>553</v>
+        <v>546</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>552</v>
+        <v>545</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="10"/>
       <c r="B41" s="6" t="s">
-        <v>555</v>
+        <v>548</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>554</v>
+        <v>547</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>609</v>
+        <v>602</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B42" s="6" t="s">
-        <v>460</v>
+        <v>453</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>556</v>
+        <v>549</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B43" s="6" t="s">
-        <v>557</v>
+        <v>550</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>558</v>
+        <v>551</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>473</v>
+        <v>466</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B44" s="6" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>559</v>
+        <v>552</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>472</v>
+        <v>465</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="10" t="s">
-        <v>509</v>
+        <v>502</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="10"/>
       <c r="B47" s="6" t="s">
-        <v>561</v>
+        <v>627</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>562</v>
+        <v>628</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>493</v>
+        <v>629</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B48" s="6" t="s">
-        <v>563</v>
+        <v>554</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>564</v>
+        <v>555</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>610</v>
+        <v>486</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B49" s="6" t="s">
-        <v>565</v>
+        <v>556</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>566</v>
+        <v>557</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>504</v>
+        <v>603</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B50" s="6" t="s">
-        <v>567</v>
+        <v>558</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>568</v>
+        <v>559</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>611</v>
+        <v>497</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B51" s="6" t="s">
-        <v>569</v>
+        <v>560</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>570</v>
+        <v>561</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="10" t="s">
-        <v>510</v>
+        <v>604</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B52" s="6" t="s">
+        <v>562</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>563</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>487</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="10"/>
-      <c r="B54" s="6" t="s">
-        <v>571</v>
-      </c>
-      <c r="C54" s="6" t="s">
-        <v>572</v>
-      </c>
-      <c r="D54" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="E54" s="6" t="s">
-        <v>474</v>
+      <c r="A54" s="10" t="s">
+        <v>503</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="10"/>
       <c r="B55" s="6" t="s">
-        <v>462</v>
+        <v>630</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>580</v>
+        <v>632</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>475</v>
+        <v>631</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="10"/>
       <c r="B56" s="6" t="s">
-        <v>573</v>
+        <v>564</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>574</v>
+        <v>565</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>503</v>
+        <v>467</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B57" s="6" t="s">
-        <v>575</v>
+        <v>455</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>480</v>
+        <v>468</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B58" s="6" t="s">
-        <v>577</v>
+        <v>566</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>581</v>
+        <v>567</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>613</v>
+        <v>496</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B59" s="6" t="s">
-        <v>578</v>
+        <v>568</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>579</v>
+        <v>569</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>471</v>
+        <v>473</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B60" s="6" t="s">
+        <v>570</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>574</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="E60" s="6" t="s">
+        <v>606</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="10" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B62" s="6" t="s">
-        <v>582</v>
-      </c>
-      <c r="C62" s="6" t="s">
-        <v>583</v>
-      </c>
-      <c r="D62" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="E62" s="6" t="s">
-        <v>489</v>
+      <c r="B61" s="6" t="s">
+        <v>571</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>572</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="E61" s="6" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B63" s="6" t="s">
-        <v>584</v>
-      </c>
-      <c r="C63" s="6" t="s">
-        <v>585</v>
-      </c>
-      <c r="D63" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="E63" s="6" t="s">
-        <v>484</v>
+      <c r="A63" s="10" t="s">
+        <v>501</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B64" s="6" t="s">
-        <v>587</v>
+        <v>575</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>586</v>
+        <v>576</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E64" s="6" t="s">
-        <v>495</v>
+        <v>482</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B65" s="6" t="s">
-        <v>590</v>
+        <v>577</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>589</v>
+        <v>578</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="E65" s="6" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="41"/>
-      <c r="B66" s="18" t="s">
-        <v>283</v>
-      </c>
-      <c r="C66" s="18" t="s">
-        <v>588</v>
-      </c>
-      <c r="D66" s="33" t="s">
-        <v>119</v>
+      <c r="B66" s="6" t="s">
+        <v>580</v>
+      </c>
+      <c r="C66" s="6" t="s">
+        <v>579</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>104</v>
       </c>
       <c r="E66" s="6" t="s">
-        <v>499</v>
+        <v>488</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="41"/>
-      <c r="B67" s="18"/>
-      <c r="C67" s="18"/>
-      <c r="D67" s="33"/>
+      <c r="B67" s="6" t="s">
+        <v>583</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>582</v>
+      </c>
+      <c r="D67" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="E67" s="6" t="s">
+        <v>472</v>
+      </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="40" t="s">
-        <v>592</v>
-      </c>
-      <c r="B68" s="18"/>
-      <c r="C68" s="18"/>
-      <c r="D68" s="33"/>
+      <c r="A68" s="41"/>
+      <c r="B68" s="18" t="s">
+        <v>277</v>
+      </c>
+      <c r="C68" s="18" t="s">
+        <v>581</v>
+      </c>
+      <c r="D68" s="33" t="s">
+        <v>114</v>
+      </c>
+      <c r="E68" s="6" t="s">
+        <v>492</v>
+      </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="40"/>
-      <c r="B69" s="18" t="s">
-        <v>593</v>
-      </c>
-      <c r="C69" s="18" t="s">
-        <v>591</v>
-      </c>
-      <c r="D69" s="33" t="s">
-        <v>107</v>
-      </c>
+      <c r="A69" s="41"/>
+      <c r="B69" s="18"/>
+      <c r="C69" s="18"/>
+      <c r="D69" s="33"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="40"/>
-      <c r="B70" s="18" t="s">
-        <v>594</v>
-      </c>
-      <c r="C70" s="18" t="s">
-        <v>603</v>
-      </c>
-      <c r="D70" s="33" t="s">
-        <v>108</v>
-      </c>
+      <c r="A70" s="40" t="s">
+        <v>585</v>
+      </c>
+      <c r="B70" s="18"/>
+      <c r="C70" s="18"/>
+      <c r="D70" s="33"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="40"/>
       <c r="B71" s="18" t="s">
-        <v>595</v>
+        <v>586</v>
       </c>
       <c r="C71" s="18" t="s">
-        <v>596</v>
+        <v>584</v>
       </c>
       <c r="D71" s="33" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="40"/>
       <c r="B72" s="18" t="s">
-        <v>597</v>
+        <v>587</v>
       </c>
       <c r="C72" s="18" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="D72" s="33" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="40"/>
       <c r="B73" s="18" t="s">
-        <v>599</v>
+        <v>588</v>
       </c>
       <c r="C73" s="18" t="s">
-        <v>602</v>
+        <v>589</v>
       </c>
       <c r="D73" s="33" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="40"/>
       <c r="B74" s="18" t="s">
-        <v>600</v>
+        <v>590</v>
       </c>
       <c r="C74" s="18" t="s">
-        <v>601</v>
+        <v>591</v>
       </c>
       <c r="D74" s="33" t="s">
-        <v>128</v>
+        <v>107</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="41"/>
-      <c r="B75" s="18"/>
-      <c r="C75" s="18"/>
-      <c r="D75" s="33"/>
+      <c r="A75" s="40"/>
+      <c r="B75" s="18" t="s">
+        <v>592</v>
+      </c>
+      <c r="C75" s="18" t="s">
+        <v>595</v>
+      </c>
+      <c r="D75" s="33" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="11" t="s">
-        <v>502</v>
+      <c r="A76" s="40"/>
+      <c r="B76" s="18" t="s">
+        <v>593</v>
+      </c>
+      <c r="C76" s="18" t="s">
+        <v>594</v>
+      </c>
+      <c r="D76" s="33" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="10"/>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="6"/>
-      <c r="D83" s="6"/>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="6"/>
-      <c r="D84" s="6"/>
+      <c r="A77" s="41"/>
+      <c r="B77" s="18"/>
+      <c r="C77" s="18"/>
+      <c r="D77" s="33"/>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="11" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="10"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="6"/>
@@ -5935,6 +6012,14 @@
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="6"/>
       <c r="D96" s="6"/>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="6"/>
+      <c r="D97" s="6"/>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="6"/>
+      <c r="D98" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>